<commit_message>
Update IP - EX 11 - Funcao SE I (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 11 - Funcao SE I (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 11 - Funcao SE I (Anexo).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8257BACD-B672-4B98-B05C-788563194A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF733787-0323-4A4A-896A-20EEB7CA758C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>EXEMPLO</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Lorenzo</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1192,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>856850</xdr:colOff>
+      <xdr:colOff>475850</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>123793</xdr:rowOff>
     </xdr:to>
@@ -1989,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q614"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,9 +2001,10 @@
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
@@ -2104,7 +2108,9 @@
       <c r="G9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="68" t="s">
+        <v>58</v>
+      </c>
       <c r="I9" s="69"/>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2124,7 +2130,10 @@
       <c r="F13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="25" t="str">
+        <f>IF(H9="Goiânia","Siga em frente!","Siga para o Retorno!")</f>
+        <v>Siga para o Retorno!</v>
+      </c>
     </row>
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2132,7 +2141,9 @@
       <c r="G17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="68"/>
+      <c r="H17" s="68">
+        <v>4</v>
+      </c>
       <c r="I17" s="69"/>
     </row>
     <row r="18" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2152,7 +2163,10 @@
       <c r="F21" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="25"/>
+      <c r="I21" s="25" t="str">
+        <f>IF(H17&lt;=4.2,"Siga em frente!","Não siga, retorne!")</f>
+        <v>Siga em frente!</v>
+      </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F22" s="17"/>
@@ -2542,7 +2556,14 @@
       <c r="D55" s="34">
         <v>49508</v>
       </c>
-      <c r="E55" s="31"/>
+      <c r="E55" s="31" t="str">
+        <f>IF($D55&gt;=I$55,"Bateu a meta!","Não bateu a meta!")</f>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F55" s="31" t="str">
+        <f>IF($D55&gt;=J$55,"Bateu a meta!","Não bateu a meta!")</f>
+        <v>Não bateu a meta!</v>
+      </c>
       <c r="H55" s="35" t="s">
         <v>33</v>
       </c>
@@ -2569,7 +2590,14 @@
       <c r="D56" s="34">
         <v>32284</v>
       </c>
-      <c r="E56" s="31"/>
+      <c r="E56" s="31" t="str">
+        <f t="shared" ref="E56:E72" si="2">IF($D56&gt;=I$55,"Bateu a meta!","Não bateu a meta!")</f>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F56" s="31" t="str">
+        <f t="shared" ref="F56:F72" si="3">IF($D56&gt;=J$55,"Bateu a meta!","Não bateu a meta!")</f>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" s="33">
@@ -2581,7 +2609,14 @@
       <c r="D57" s="34">
         <v>35019</v>
       </c>
-      <c r="E57" s="31"/>
+      <c r="E57" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F57" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" s="33">
@@ -2593,7 +2628,14 @@
       <c r="D58" s="34">
         <v>41551</v>
       </c>
-      <c r="E58" s="31"/>
+      <c r="E58" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F58" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="33">
@@ -2605,7 +2647,14 @@
       <c r="D59" s="34">
         <v>41334</v>
       </c>
-      <c r="E59" s="31"/>
+      <c r="E59" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F59" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="33">
@@ -2617,7 +2666,14 @@
       <c r="D60" s="34">
         <v>43163</v>
       </c>
-      <c r="E60" s="31"/>
+      <c r="E60" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F60" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="61" spans="2:17" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="33">
@@ -2629,7 +2685,14 @@
       <c r="D61" s="34">
         <v>43412</v>
       </c>
-      <c r="E61" s="31"/>
+      <c r="E61" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F61" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61"/>
@@ -2649,7 +2712,14 @@
       <c r="D62" s="34">
         <v>31852</v>
       </c>
-      <c r="E62" s="31"/>
+      <c r="E62" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F62" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="33">
@@ -2661,7 +2731,14 @@
       <c r="D63" s="34">
         <v>33700</v>
       </c>
-      <c r="E63" s="31"/>
+      <c r="E63" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F63" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="33">
@@ -2673,9 +2750,16 @@
       <c r="D64" s="34">
         <v>33572</v>
       </c>
-      <c r="E64" s="31"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F64" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="33">
         <v>1016</v>
       </c>
@@ -2685,9 +2769,16 @@
       <c r="D65" s="34">
         <v>33386</v>
       </c>
-      <c r="E65" s="31"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F65" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="33">
         <v>1015</v>
       </c>
@@ -2697,9 +2788,16 @@
       <c r="D66" s="34">
         <v>44632</v>
       </c>
-      <c r="E66" s="31"/>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F66" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="33">
         <v>1018</v>
       </c>
@@ -2709,9 +2807,16 @@
       <c r="D67" s="34">
         <v>46654</v>
       </c>
-      <c r="E67" s="31"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F67" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="33">
         <v>1001</v>
       </c>
@@ -2721,9 +2826,16 @@
       <c r="D68" s="34">
         <v>30745</v>
       </c>
-      <c r="E68" s="31"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F68" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="33">
         <v>1004</v>
       </c>
@@ -2733,9 +2845,16 @@
       <c r="D69" s="34">
         <v>41812</v>
       </c>
-      <c r="E69" s="31"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F69" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="33">
         <v>1012</v>
       </c>
@@ -2745,9 +2864,16 @@
       <c r="D70" s="34">
         <v>32740</v>
       </c>
-      <c r="E70" s="31"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F70" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="33">
         <v>1002</v>
       </c>
@@ -2757,9 +2883,16 @@
       <c r="D71" s="34">
         <v>38543</v>
       </c>
-      <c r="E71" s="31"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Não bateu a meta!</v>
+      </c>
+      <c r="F71" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="33">
         <v>1013</v>
       </c>
@@ -2769,37 +2902,44 @@
       <c r="D72" s="34">
         <v>43686</v>
       </c>
-      <c r="E72" s="31"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="31" t="str">
+        <f t="shared" si="2"/>
+        <v>Bateu a meta!</v>
+      </c>
+      <c r="F72" s="31" t="str">
+        <f t="shared" si="3"/>
+        <v>Não bateu a meta!</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D73" s="30"/>
       <c r="E73" s="31"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D74" s="30"/>
       <c r="E74" s="31"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D75" s="30"/>
       <c r="E75" s="31"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D76" s="30"/>
       <c r="E76" s="31"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D77" s="30"/>
       <c r="E77" s="31"/>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D78" s="30"/>
       <c r="E78" s="31"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D79" s="30"/>
       <c r="E79" s="31"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D80" s="30"/>
       <c r="E80" s="31"/>
     </row>

</xml_diff>